<commit_message>
Switch to using string type for searches
</commit_message>
<xml_diff>
--- a/config/default/forms/app/pregnancy.xlsx
+++ b/config/default/forms/app/pregnancy.xlsx
@@ -172,7 +172,7 @@
     <t xml:space="preserve">Contact ID</t>
   </si>
   <si>
-    <t xml:space="preserve">select-contact person</t>
+    <t xml:space="preserve">select-contact type-person</t>
   </si>
   <si>
     <t xml:space="preserve">parent</t>
@@ -2960,7 +2960,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L161" activeCellId="0" sqref="L161"/>
+      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2980,7 +2980,7 @@
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="20" min="15" style="0" width="25.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="73.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="24" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="31" style="0" width="29.86"/>
@@ -17298,7 +17298,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
@@ -17355,7 +17355,7 @@
       </c>
       <c r="C2" s="57" t="n">
         <f aca="true">NOW()</f>
-        <v>43963.6420593429</v>
+        <v>43965.5587619736</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>678</v>

</xml_diff>

<commit_message>
Just use string type...
</commit_message>
<xml_diff>
--- a/config/default/forms/app/pregnancy.xlsx
+++ b/config/default/forms/app/pregnancy.xlsx
@@ -163,7 +163,7 @@
     <t xml:space="preserve">User</t>
   </si>
   <si>
-    <t xml:space="preserve">select-contact</t>
+    <t xml:space="preserve">string</t>
   </si>
   <si>
     <t xml:space="preserve">contact_id</t>
@@ -2960,7 +2960,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17355,7 +17355,7 @@
       </c>
       <c r="C2" s="57" t="n">
         <f aca="true">NOW()</f>
-        <v>43965.5587619736</v>
+        <v>43965.5754322576</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>678</v>

</xml_diff>

<commit_message>
Update the default xlsx
</commit_message>
<xml_diff>
--- a/config/default/forms/app/pregnancy.xlsx
+++ b/config/default/forms/app/pregnancy.xlsx
@@ -2960,7 +2960,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17355,7 +17355,7 @@
       </c>
       <c r="C2" s="57" t="n">
         <f aca="true">NOW()</f>
-        <v>43965.5754322576</v>
+        <v>43966.3899077575</v>
       </c>
       <c r="D2" s="56" t="s">
         <v>678</v>

</xml_diff>